<commit_message>
save current progress before pushing to GitHub
</commit_message>
<xml_diff>
--- a/data/ac_dc_real_case.xlsx
+++ b/data/ac_dc_real_case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13380" firstSheet="9" activeTab="19"/>
+    <workbookView windowWidth="28800" windowHeight="13380" firstSheet="10" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="cable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="550">
   <si>
     <t>Index</t>
   </si>
@@ -1642,6 +1642,9 @@
   </si>
   <si>
     <t>Battery4</t>
+  </si>
+  <si>
+    <t>Battery5</t>
   </si>
   <si>
     <t>EFF100</t>
@@ -7451,13 +7454,13 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AK5"/>
+  <dimension ref="A1:AK6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
     <col min="16" max="16" width="11.5"/>
     <col min="21" max="21" width="12.625"/>
@@ -8025,6 +8028,119 @@
         <v>531</v>
       </c>
       <c r="AK5" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>536</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>85</v>
+      </c>
+      <c r="F6" s="2">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="2">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2">
+        <v>20</v>
+      </c>
+      <c r="M6" s="2">
+        <v>20</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>100</v>
+      </c>
+      <c r="P6" s="2">
+        <v>2185560065</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>3220</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.00100000005</v>
+      </c>
+      <c r="S6" s="2">
+        <v>1</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0.00100000005</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0.100000001</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0</v>
+      </c>
+      <c r="W6" s="2">
+        <v>110</v>
+      </c>
+      <c r="X6" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>120</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>100</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>531</v>
+      </c>
+      <c r="AK6" t="s">
         <v>532</v>
       </c>
     </row>
@@ -8053,13 +8169,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -8074,13 +8190,13 @@
         <v>314</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>205</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>318</v>
@@ -8104,19 +8220,19 @@
         <v>327</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>229</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>231</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>329</v>
@@ -8125,19 +8241,19 @@
         <v>330</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>157</v>
@@ -8155,7 +8271,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -9610,7 +9726,7 @@
   <sheetPr/>
   <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" topLeftCell="O1" workbookViewId="0">
       <selection activeCell="R61" sqref="R61"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: adaptive cumulative probability detection for MC and cluster export
</commit_message>
<xml_diff>
--- a/data/ac_dc_real_case.xlsx
+++ b/data/ac_dc_real_case.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="554">
   <si>
     <t>Index</t>
   </si>
@@ -1638,13 +1638,25 @@
     <t>Battery2</t>
   </si>
   <si>
+    <t>Bus_观龙20队公变1</t>
+  </si>
+  <si>
     <t>Battery3</t>
   </si>
   <si>
+    <t>Bus_观龙大站2A公变房1</t>
+  </si>
+  <si>
     <t>Battery4</t>
   </si>
   <si>
+    <t>Bus_观龙大站公变房#1变压器1</t>
+  </si>
+  <si>
     <t>Battery5</t>
+  </si>
+  <si>
+    <t>Bus_观龙村19队2号#1公变1</t>
   </si>
   <si>
     <t>EFF100</t>
@@ -7457,7 +7469,7 @@
   <dimension ref="A1:AK6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -7721,7 +7733,7 @@
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>534</v>
       </c>
       <c r="K3" s="2">
         <v>20</v>
@@ -7810,7 +7822,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -7834,7 +7846,7 @@
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>61</v>
+        <v>536</v>
       </c>
       <c r="K4" s="2">
         <v>20</v>
@@ -7923,7 +7935,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -7947,7 +7959,7 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>538</v>
       </c>
       <c r="K5" s="2">
         <v>20</v>
@@ -8036,7 +8048,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -8060,7 +8072,7 @@
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>540</v>
       </c>
       <c r="K6" s="2">
         <v>20</v>
@@ -8169,13 +8181,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -8190,13 +8202,13 @@
         <v>314</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>205</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>318</v>
@@ -8220,19 +8232,19 @@
         <v>327</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>229</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>231</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>329</v>
@@ -8241,19 +8253,19 @@
         <v>330</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>157</v>

</xml_diff>

<commit_message>
Update all modified files in the repository
</commit_message>
<xml_diff>
--- a/data/ac_dc_real_case.xlsx
+++ b/data/ac_dc_real_case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13380" firstSheet="10" activeTab="19"/>
+    <workbookView windowWidth="28800" windowHeight="13380" firstSheet="9" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="cable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="550">
   <si>
     <t>Index</t>
   </si>
@@ -1629,9 +1629,6 @@
     <t>Battery1</t>
   </si>
   <si>
-    <t>Bus_大刀沙村2号直流1</t>
-  </si>
-  <si>
     <t>450043002D003200300030003700200020002000200020000000000000003041443730333430762F000030304330373934343030303030303030190008000000</t>
   </si>
   <si>
@@ -1641,25 +1638,13 @@
     <t>Battery2</t>
   </si>
   <si>
-    <t>Bus_观龙20队公变1</t>
-  </si>
-  <si>
     <t>Battery3</t>
   </si>
   <si>
-    <t>Bus_观龙大站2A公变房1</t>
-  </si>
-  <si>
     <t>Battery4</t>
   </si>
   <si>
-    <t>Bus_观龙大站公变房#1变压器1</t>
-  </si>
-  <si>
     <t>Battery5</t>
-  </si>
-  <si>
-    <t>Bus_观龙村19队2号#1公变1</t>
   </si>
   <si>
     <t>EFF100</t>
@@ -2784,7 +2769,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:D27"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7472,7 +7457,7 @@
   <dimension ref="A1:AK6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -7623,7 +7608,7 @@
         <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>531</v>
+        <v>298</v>
       </c>
       <c r="K2" s="2">
         <v>20</v>
@@ -7701,10 +7686,10 @@
         <v>0</v>
       </c>
       <c r="AJ2" t="s">
+        <v>531</v>
+      </c>
+      <c r="AK2" t="s">
         <v>532</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="3" spans="1:37">
@@ -7712,7 +7697,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
@@ -7736,7 +7721,7 @@
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>535</v>
+        <v>65</v>
       </c>
       <c r="K3" s="2">
         <v>20</v>
@@ -7814,10 +7799,10 @@
         <v>0</v>
       </c>
       <c r="AJ3" t="s">
+        <v>531</v>
+      </c>
+      <c r="AK3" t="s">
         <v>532</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:37">
@@ -7825,7 +7810,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -7849,7 +7834,7 @@
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>537</v>
+        <v>61</v>
       </c>
       <c r="K4" s="2">
         <v>20</v>
@@ -7927,10 +7912,10 @@
         <v>0</v>
       </c>
       <c r="AJ4" t="s">
+        <v>531</v>
+      </c>
+      <c r="AK4" t="s">
         <v>532</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="5" spans="1:37">
@@ -7938,7 +7923,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -7962,7 +7947,7 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>539</v>
+        <v>63</v>
       </c>
       <c r="K5" s="2">
         <v>20</v>
@@ -8040,10 +8025,10 @@
         <v>0</v>
       </c>
       <c r="AJ5" t="s">
+        <v>531</v>
+      </c>
+      <c r="AK5" t="s">
         <v>532</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -8051,7 +8036,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -8075,7 +8060,7 @@
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>541</v>
+        <v>57</v>
       </c>
       <c r="K6" s="2">
         <v>20</v>
@@ -8153,10 +8138,10 @@
         <v>0</v>
       </c>
       <c r="AJ6" t="s">
+        <v>531</v>
+      </c>
+      <c r="AK6" t="s">
         <v>532</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -8184,13 +8169,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -8205,13 +8190,13 @@
         <v>314</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>205</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>318</v>
@@ -8235,19 +8220,19 @@
         <v>327</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>229</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>231</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>329</v>
@@ -8256,19 +8241,19 @@
         <v>330</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>157</v>

</xml_diff>